<commit_message>
Device control: auto mode by model and sensors taking watering duration
</commit_message>
<xml_diff>
--- a/Files/calculations.xlsx
+++ b/Files/calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="5250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="5250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Solenoids" sheetId="2" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="179">
   <si>
     <t>Raspberry</t>
   </si>
@@ -441,18 +441,205 @@
   </si>
   <si>
     <t>+3 opened'</t>
+  </si>
+  <si>
+    <t>m soil, g</t>
+  </si>
+  <si>
+    <t>r, cm</t>
+  </si>
+  <si>
+    <t>h, cm</t>
+  </si>
+  <si>
+    <t>d, cm</t>
+  </si>
+  <si>
+    <t>S pot,  cm2</t>
+  </si>
+  <si>
+    <t>ρ soil, g/cm3</t>
+  </si>
+  <si>
+    <t>const</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>rain (mm)</t>
+  </si>
+  <si>
+    <t>showers (mm)</t>
+  </si>
+  <si>
+    <t>Whether API</t>
+  </si>
+  <si>
+    <t>= h of added water, cm</t>
+  </si>
+  <si>
+    <t>= V of  added water, cm3</t>
+  </si>
+  <si>
+    <t>V soil, l (=1000 cm3)</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>= actual % hum</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>= need % hum</t>
+  </si>
+  <si>
+    <t>m water for 100% hum, g</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>cm3 (=ml)</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>water, g (=ml)</t>
+  </si>
+  <si>
+    <t>ml/s</t>
+  </si>
+  <si>
+    <t>debit sol, ml/s</t>
+  </si>
+  <si>
+    <t>diff (need to add), ml</t>
+  </si>
+  <si>
+    <t>t  opening of sol, s</t>
+  </si>
+  <si>
+    <t>Arrosage basing on sensors</t>
+  </si>
+  <si>
+    <t>Arrosage basing on model</t>
+  </si>
+  <si>
+    <t>water, %</t>
+  </si>
+  <si>
+    <t>cactus</t>
+  </si>
+  <si>
+    <t>rose</t>
+  </si>
+  <si>
+    <t>petunia</t>
+  </si>
+  <si>
+    <t>per day 40 deg, ml</t>
+  </si>
+  <si>
+    <t>per day 20 deg, ml</t>
+  </si>
+  <si>
+    <t>скорость потребления воды в день растением в зависимости от</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - температуры</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - категории</t>
+  </si>
+  <si>
+    <t>10 deg, ml</t>
+  </si>
+  <si>
+    <t>20 deg, ml</t>
+  </si>
+  <si>
+    <t>30 deg, ml</t>
+  </si>
+  <si>
+    <t>40 deg, ml</t>
+  </si>
+  <si>
+    <t>сколько надо растению</t>
+  </si>
+  <si>
+    <t>воды в день</t>
+  </si>
+  <si>
+    <t>в зависимости от температуры</t>
+  </si>
+  <si>
+    <t>t за прошлый день</t>
+  </si>
+  <si>
+    <t>осадки за прошлый день</t>
+  </si>
+  <si>
+    <t>50 deg, ml</t>
+  </si>
+  <si>
+    <t>need water for this t</t>
+  </si>
+  <si>
+    <t>S, cm2</t>
+  </si>
+  <si>
+    <t>V soil, cm3</t>
+  </si>
+  <si>
+    <t>add to Flowerpot</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>cat1</t>
+  </si>
+  <si>
+    <t>cat2</t>
+  </si>
+  <si>
+    <t>cat3</t>
+  </si>
+  <si>
+    <t>data from DB  -&gt;</t>
+  </si>
+  <si>
+    <t>d, cm2</t>
+  </si>
+  <si>
+    <t>mass, g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,6 +749,45 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -753,7 +979,7 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -857,7 +1083,6 @@
     <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -873,6 +1098,59 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% — акцент1" xfId="3" builtinId="30"/>
@@ -2157,7 +2435,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2608,7 +2885,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4104,8 +4380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:C36"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5153,11 +5429,11 @@
       <c r="A33" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="70">
+      <c r="B33" s="69">
         <f>0.1/C10</f>
         <v>2.1739130434782612E-2</v>
       </c>
-      <c r="C33" s="72">
+      <c r="C33" s="71">
         <f>B33*3</f>
         <v>6.5217391304347838E-2</v>
       </c>
@@ -5166,11 +5442,11 @@
       <c r="A34" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="70">
+      <c r="B34" s="69">
         <f>0.1/D10</f>
         <v>2.5641025641025644E-2</v>
       </c>
-      <c r="C34" s="72">
+      <c r="C34" s="71">
         <f t="shared" ref="C34:C36" si="21">B34*3</f>
         <v>7.6923076923076927E-2</v>
       </c>
@@ -5179,11 +5455,11 @@
       <c r="A35" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="70">
+      <c r="B35" s="69">
         <f>0.1/E10</f>
         <v>2.777777777777778E-2</v>
       </c>
-      <c r="C35" s="72">
+      <c r="C35" s="71">
         <f t="shared" si="21"/>
         <v>8.3333333333333343E-2</v>
       </c>
@@ -5192,20 +5468,20 @@
       <c r="A36" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="70">
+      <c r="B36" s="69">
         <f>0.1/F10</f>
         <v>2.3809523809523808E-2</v>
       </c>
-      <c r="C36" s="72">
+      <c r="C36" s="71">
         <f t="shared" si="21"/>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="71" t="s">
+      <c r="B37" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="C37" s="71" t="s">
+      <c r="C37" s="70" t="s">
         <v>116</v>
       </c>
     </row>
@@ -5218,17 +5494,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:X25"/>
+  <dimension ref="A2:X59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" style="19" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="19" customWidth="1"/>
     <col min="6" max="6" width="19" style="19" customWidth="1"/>
@@ -5300,6 +5576,10 @@
         <f>O7/(Solenoids!Q8/10)</f>
         <v>10.399893326221747</v>
       </c>
+      <c r="P3" s="81">
+        <f>O3+M3+K3+I3+G3</f>
+        <v>34.666311087405823</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G4" s="54" t="s">
@@ -5597,7 +5877,7 @@
       <c r="O15" s="47"/>
       <c r="P15" s="48"/>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N17" s="19" t="s">
         <v>99</v>
       </c>
@@ -5606,29 +5886,29 @@
         <v>551.19434628975262</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O18" s="44">
         <f>D8*B8</f>
         <v>388.24204946996468</v>
       </c>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C19" s="19"/>
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="64" t="s">
+      <c r="E19" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="64" t="s">
+      <c r="F19" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="G19" s="64" t="s">
+      <c r="G19" s="63" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="67" t="s">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="66" t="s">
         <v>108</v>
       </c>
       <c r="D20" s="19">
@@ -5644,8 +5924,8 @@
         <v>695</v>
       </c>
     </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="67" t="s">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="66" t="s">
         <v>109</v>
       </c>
       <c r="D21" s="19">
@@ -5660,38 +5940,644 @@
       <c r="G21" s="19">
         <v>321</v>
       </c>
-      <c r="I21" s="63"/>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C22" s="66" t="s">
+      <c r="I21" s="62"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C22" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="64">
         <f>D21/D20</f>
         <v>0.41847041847041849</v>
       </c>
-      <c r="E22" s="65">
+      <c r="E22" s="64">
         <f t="shared" ref="E22:G22" si="0">E21/E20</f>
         <v>0.46656050955414013</v>
       </c>
-      <c r="F22" s="65">
+      <c r="F22" s="64">
         <f t="shared" si="0"/>
         <v>0.46296296296296297</v>
       </c>
-      <c r="G22" s="65">
+      <c r="G22" s="64">
         <f t="shared" si="0"/>
         <v>0.46187050359712228</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C23" s="19"/>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D24" s="61"/>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="F25" s="62"/>
-      <c r="J25" s="62"/>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D24" s="76" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="I24" s="76" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D25" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="63" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="H25" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="I25" s="72" t="s">
+        <v>120</v>
+      </c>
+      <c r="J25" s="72" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D26" s="55">
+        <v>3</v>
+      </c>
+      <c r="E26" s="55">
+        <v>1300</v>
+      </c>
+      <c r="F26" s="73">
+        <f>E26/D27</f>
+        <v>0.47272727272727272</v>
+      </c>
+      <c r="G26" s="55">
+        <v>16</v>
+      </c>
+      <c r="H26" s="73">
+        <f>SQRT(D27/(PI()*G26))</f>
+        <v>7.3965878408789969</v>
+      </c>
+      <c r="I26" s="73">
+        <f>H26*2</f>
+        <v>14.793175681757994</v>
+      </c>
+      <c r="J26" s="73">
+        <f>PI()*I26*I26/4</f>
+        <v>171.875</v>
+      </c>
+      <c r="K26" s="73"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D27" s="55">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F28" s="19">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="J28" s="19">
+        <v>10</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="L28" s="75" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I29" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="J29" s="19">
+        <v>15</v>
+      </c>
+      <c r="K29" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="L29" s="75" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D30" s="63"/>
+      <c r="E30" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H30" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="I30" s="77"/>
+      <c r="J30" s="19">
+        <f>(J29+J28)/10</f>
+        <v>2.5</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E31" s="19">
+        <f>E26*1.09</f>
+        <v>1417</v>
+      </c>
+      <c r="H31" s="79" t="s">
+        <v>129</v>
+      </c>
+      <c r="I31" s="79"/>
+      <c r="J31" s="22">
+        <f>PI()*H26*H26*J30</f>
+        <v>429.6875</v>
+      </c>
+      <c r="K31" s="80" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="99" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" s="100" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="100" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" s="100" t="s">
+        <v>177</v>
+      </c>
+      <c r="E32" s="101" t="s">
+        <v>119</v>
+      </c>
+      <c r="F32" s="101" t="s">
+        <v>178</v>
+      </c>
+      <c r="H32" s="77"/>
+      <c r="J32" s="74"/>
+      <c r="K32" s="61"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="91">
+        <v>1</v>
+      </c>
+      <c r="B33" s="102">
+        <f>6000</f>
+        <v>6000</v>
+      </c>
+      <c r="C33" s="98">
+        <f>PI()*D33*D33/4</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="D33" s="61">
+        <v>20</v>
+      </c>
+      <c r="E33" s="74">
+        <f>12*B33/(PI()*D33*D33)</f>
+        <v>57.295779513082323</v>
+      </c>
+      <c r="F33" s="74">
+        <f>B33*F26</f>
+        <v>2836.3636363636365</v>
+      </c>
+      <c r="G33" s="82"/>
+      <c r="H33" s="83" t="s">
+        <v>145</v>
+      </c>
+      <c r="I33" s="84"/>
+      <c r="J33" s="85"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="84"/>
+      <c r="M33" s="87"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="91">
+        <v>2</v>
+      </c>
+      <c r="B34" s="102">
+        <v>800</v>
+      </c>
+      <c r="C34" s="98">
+        <f t="shared" ref="C34:C36" si="1">PI()*D34*D34/4</f>
+        <v>113.09733552923255</v>
+      </c>
+      <c r="D34" s="19">
+        <v>12</v>
+      </c>
+      <c r="E34" s="74">
+        <f>12*B34/(PI()*D34*D34)</f>
+        <v>21.220659078919379</v>
+      </c>
+      <c r="F34" s="74">
+        <f>B34*F26</f>
+        <v>378.18181818181819</v>
+      </c>
+      <c r="G34" s="18"/>
+      <c r="J34" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="M34" s="20"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="91">
+        <v>3</v>
+      </c>
+      <c r="B35" s="102">
+        <v>1200</v>
+      </c>
+      <c r="C35" s="98">
+        <f t="shared" si="1"/>
+        <v>153.93804002589985</v>
+      </c>
+      <c r="D35" s="61">
+        <v>14</v>
+      </c>
+      <c r="E35" s="74">
+        <f t="shared" ref="E34:E36" si="2">12*B35/(PI()*D35*D35)</f>
+        <v>23.386032454319317</v>
+      </c>
+      <c r="F35" s="74">
+        <f>B35*F26</f>
+        <v>567.27272727272725</v>
+      </c>
+      <c r="G35" s="18"/>
+      <c r="H35" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="J35" s="19">
+        <v>20</v>
+      </c>
+      <c r="K35" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="L35" s="19">
+        <f>E31*J35/100</f>
+        <v>283.39999999999998</v>
+      </c>
+      <c r="M35" s="20"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="91">
+        <v>4</v>
+      </c>
+      <c r="B36" s="102">
+        <v>4800</v>
+      </c>
+      <c r="C36" s="98">
+        <f t="shared" si="1"/>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="D36" s="61">
+        <v>20</v>
+      </c>
+      <c r="E36" s="74">
+        <f t="shared" si="2"/>
+        <v>45.836623610465857</v>
+      </c>
+      <c r="F36" s="74">
+        <f>B36*F26</f>
+        <v>2269.090909090909</v>
+      </c>
+      <c r="G36" s="18"/>
+      <c r="H36" s="78" t="s">
+        <v>135</v>
+      </c>
+      <c r="J36" s="19">
+        <v>50</v>
+      </c>
+      <c r="K36" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="L36" s="19">
+        <f>E31*J36/100</f>
+        <v>708.5</v>
+      </c>
+      <c r="M36" s="20"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G37" s="18"/>
+      <c r="H37" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22">
+        <f>L36-L35</f>
+        <v>425.1</v>
+      </c>
+      <c r="M37" s="20"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F38"/>
+      <c r="G38" s="18"/>
+      <c r="M38" s="20"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D39" s="44"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="L39" s="74">
+        <f>L37/J40</f>
+        <v>92.413043478260889</v>
+      </c>
+      <c r="M39" s="20"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D40" s="44"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="88" t="s">
+        <v>142</v>
+      </c>
+      <c r="I40" s="88"/>
+      <c r="J40" s="88">
+        <f>Solenoids!C10</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K40" s="88" t="s">
+        <v>141</v>
+      </c>
+      <c r="L40" s="88"/>
+      <c r="M40" s="48"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D41" s="44"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D42" s="44"/>
+      <c r="H42" s="79" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D43" s="44"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D44" s="44"/>
+      <c r="G44" s="61" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D45" s="44"/>
+      <c r="G45" s="77" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D46" s="44"/>
+      <c r="G46" s="77" t="s">
+        <v>155</v>
+      </c>
+      <c r="J46" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="K46" s="22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H47" s="19">
+        <v>1</v>
+      </c>
+      <c r="I47" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="J47" s="1">
+        <f>237/(2*7)</f>
+        <v>16.928571428571427</v>
+      </c>
+      <c r="K47" s="74">
+        <f>237/(4*7)</f>
+        <v>8.4642857142857135</v>
+      </c>
+      <c r="L47" s="89">
+        <f>J47/K47</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H48" s="19">
+        <v>2</v>
+      </c>
+      <c r="I48" s="61" t="s">
+        <v>150</v>
+      </c>
+      <c r="J48" s="74">
+        <f>4000/7</f>
+        <v>571.42857142857144</v>
+      </c>
+      <c r="K48" s="74">
+        <f>2000/7</f>
+        <v>285.71428571428572</v>
+      </c>
+      <c r="L48" s="89">
+        <f t="shared" ref="L48:L49" si="3">J48/K48</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="H49" s="19">
+        <v>3</v>
+      </c>
+      <c r="I49" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="J49" s="74">
+        <f>5000/7</f>
+        <v>714.28571428571433</v>
+      </c>
+      <c r="K49" s="74">
+        <f>3000/7</f>
+        <v>428.57142857142856</v>
+      </c>
+      <c r="L49" s="89">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="N49" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="O49" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="P49" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="I50" s="61"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
+      <c r="L50" s="89"/>
+    </row>
+    <row r="51" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="H51" s="92"/>
+      <c r="I51" s="93" t="s">
+        <v>156</v>
+      </c>
+      <c r="J51" s="94" t="s">
+        <v>157</v>
+      </c>
+      <c r="K51" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="L51" s="93" t="s">
+        <v>159</v>
+      </c>
+      <c r="M51" s="93" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F52" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="H52" s="96" t="s">
+        <v>173</v>
+      </c>
+      <c r="I52" s="95">
+        <f>J52/2</f>
+        <v>4.2321428571428568</v>
+      </c>
+      <c r="J52" s="95">
+        <f>K47</f>
+        <v>8.4642857142857135</v>
+      </c>
+      <c r="K52" s="95">
+        <f>(J52+L52)/2</f>
+        <v>12.696428571428569</v>
+      </c>
+      <c r="L52" s="95">
+        <f>J47</f>
+        <v>16.928571428571427</v>
+      </c>
+      <c r="M52" s="95">
+        <f>K52*2</f>
+        <v>25.392857142857139</v>
+      </c>
+    </row>
+    <row r="53" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F53" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="H53" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="I53" s="95">
+        <f t="shared" ref="I53:I54" si="4">J53/2</f>
+        <v>142.85714285714286</v>
+      </c>
+      <c r="J53" s="95">
+        <f>K48</f>
+        <v>285.71428571428572</v>
+      </c>
+      <c r="K53" s="95">
+        <f>(J53+L53)/2</f>
+        <v>428.57142857142856</v>
+      </c>
+      <c r="L53" s="95">
+        <f>J48</f>
+        <v>571.42857142857144</v>
+      </c>
+      <c r="M53" s="95">
+        <f t="shared" ref="M53" si="5">K53*2</f>
+        <v>857.14285714285711</v>
+      </c>
+    </row>
+    <row r="54" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F54" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="H54" s="97" t="s">
+        <v>175</v>
+      </c>
+      <c r="I54" s="95">
+        <f t="shared" si="4"/>
+        <v>214.28571428571428</v>
+      </c>
+      <c r="J54" s="95">
+        <f>K49</f>
+        <v>428.57142857142856</v>
+      </c>
+      <c r="K54" s="95">
+        <f t="shared" ref="K54" si="6">(J54+L54)/2</f>
+        <v>571.42857142857144</v>
+      </c>
+      <c r="L54" s="95">
+        <f>J49</f>
+        <v>714.28571428571433</v>
+      </c>
+      <c r="M54" s="95">
+        <f>K54*2</f>
+        <v>1142.8571428571429</v>
+      </c>
+    </row>
+    <row r="56" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F56" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="H56" s="79" t="s">
+        <v>129</v>
+      </c>
+      <c r="I56" s="79"/>
+      <c r="J56" s="22">
+        <f>J31</f>
+        <v>429.6875</v>
+      </c>
+      <c r="K56" s="80" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F57" s="61" t="s">
+        <v>163</v>
+      </c>
+      <c r="J57" s="19">
+        <v>27</v>
+      </c>
+      <c r="L57" s="75" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F58" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H58" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="I58" s="22"/>
+      <c r="J58" s="90">
+        <f>(K54-J54)*(J57-20)/(30-20)+J54</f>
+        <v>528.57142857142856</v>
+      </c>
+      <c r="K58" s="22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="H59" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="I59" s="22"/>
+      <c r="J59" s="90">
+        <f>J58-J56</f>
+        <v>98.883928571428555</v>
+      </c>
+      <c r="K59" s="22" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5703,8 +6589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5783,7 +6669,7 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="67" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="11">
@@ -5792,16 +6678,16 @@
       <c r="D8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="67">
         <v>14</v>
       </c>
-      <c r="F8" s="69">
+      <c r="F8" s="68">
         <f>Solenoids!F10</f>
         <v>4.2</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="67" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="11">
@@ -5810,16 +6696,16 @@
       <c r="D9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="67">
         <v>22</v>
       </c>
-      <c r="F9" s="69">
+      <c r="F9" s="68">
         <f>Solenoids!E10</f>
         <v>3.6</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="67" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="11">
@@ -5828,16 +6714,16 @@
       <c r="D10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="68">
+      <c r="E10" s="67">
         <v>27</v>
       </c>
-      <c r="F10" s="69">
+      <c r="F10" s="68">
         <f>Solenoids!D10</f>
         <v>3.9</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="67" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="11">
@@ -5846,10 +6732,10 @@
       <c r="D11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="68">
+      <c r="E11" s="67">
         <v>17</v>
       </c>
-      <c r="F11" s="69">
+      <c r="F11" s="68">
         <f>Solenoids!C10</f>
         <v>4.5999999999999996</v>
       </c>
@@ -5869,58 +6755,58 @@
       </c>
     </row>
     <row r="15" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="68">
+      <c r="C15" s="67">
         <v>0</v>
       </c>
-      <c r="D15" s="68">
+      <c r="D15" s="67">
         <v>290</v>
       </c>
-      <c r="E15" s="69">
+      <c r="E15" s="68">
         <v>693</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="68">
+      <c r="C16" s="67">
         <v>1</v>
       </c>
-      <c r="D16" s="68">
+      <c r="D16" s="67">
         <v>293</v>
       </c>
-      <c r="E16" s="69">
+      <c r="E16" s="68">
         <v>628</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="68">
+      <c r="C17" s="67">
         <v>2</v>
       </c>
-      <c r="D17" s="68">
+      <c r="D17" s="67">
         <v>375</v>
       </c>
-      <c r="E17" s="69">
+      <c r="E17" s="68">
         <v>810</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="68">
+      <c r="C18" s="67">
         <v>3</v>
       </c>
-      <c r="D18" s="68">
+      <c r="D18" s="67">
         <v>321</v>
       </c>
-      <c r="E18" s="69">
+      <c r="E18" s="68">
         <v>695</v>
       </c>
     </row>

</xml_diff>